<commit_message>
ECB May 2025 update
</commit_message>
<xml_diff>
--- a/ECB_mean.xlsx
+++ b/ECB_mean.xlsx
@@ -69,7 +69,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -112,7 +112,7 @@
         <v>43922</v>
       </c>
       <c r="B5" s="2">
-        <v>3.5908604876194468</v>
+        <v>3.5908604878022601</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -123,7 +123,7 @@
         <v>43952</v>
       </c>
       <c r="B6" s="2">
-        <v>3.8008905492715899</v>
+        <v>3.8008905500200849</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -134,7 +134,7 @@
         <v>43983</v>
       </c>
       <c r="B7" s="2">
-        <v>3.6810664046212551</v>
+        <v>3.6810664065035921</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -156,7 +156,7 @@
         <v>44044</v>
       </c>
       <c r="B9" s="2">
-        <v>3.0374057490289874</v>
+        <v>3.0374057487693267</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -167,7 +167,7 @@
         <v>44075</v>
       </c>
       <c r="B10" s="2">
-        <v>2.8325894072586886</v>
+        <v>2.8325894070830571</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -178,7 +178,7 @@
         <v>44105</v>
       </c>
       <c r="B11" s="2">
-        <v>3.454631765499617</v>
+        <v>3.4546317652178429</v>
       </c>
       <c r="C11" s="2">
         <v>2.3499999046325684</v>
@@ -200,7 +200,7 @@
         <v>44166</v>
       </c>
       <c r="B13" s="2">
-        <v>3.5720210699628878</v>
+        <v>3.572021069962886</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -244,7 +244,7 @@
         <v>44287</v>
       </c>
       <c r="B17" s="2">
-        <v>3.5242325153881962</v>
+        <v>3.5242325153881935</v>
       </c>
       <c r="C17" s="2">
         <v>2.0999999046325684</v>
@@ -258,7 +258,7 @@
         <v>3.3112868904116803</v>
       </c>
       <c r="C18" s="2">
-        <v>2.1500000953674317</v>
+        <v>2.1500000953674316</v>
       </c>
     </row>
     <row r="19">
@@ -299,7 +299,7 @@
         <v>44440</v>
       </c>
       <c r="B22" s="2">
-        <v>3.9802982039355532</v>
+        <v>3.9802982039355528</v>
       </c>
       <c r="C22" s="2">
         <v>3</v>
@@ -310,7 +310,7 @@
         <v>44470</v>
       </c>
       <c r="B23" s="2">
-        <v>3.8307683254914466</v>
+        <v>3.8307683257712619</v>
       </c>
       <c r="C23" s="2">
         <v>2.2999999523162842</v>
@@ -321,7 +321,7 @@
         <v>44501</v>
       </c>
       <c r="B24" s="2">
-        <v>5.3954159363957173</v>
+        <v>5.395415937067412</v>
       </c>
       <c r="C24" s="2">
         <v>4.3500003814697266</v>
@@ -332,7 +332,7 @@
         <v>44531</v>
       </c>
       <c r="B25" s="2">
-        <v>4.1723447530747091</v>
+        <v>4.17234475307471</v>
       </c>
       <c r="C25" s="2">
         <v>3</v>
@@ -343,7 +343,7 @@
         <v>44562</v>
       </c>
       <c r="B26" s="2">
-        <v>4.906882975223958</v>
+        <v>4.9068829752239349</v>
       </c>
       <c r="C26" s="2">
         <v>4.5999999046325684</v>
@@ -376,7 +376,7 @@
         <v>44652</v>
       </c>
       <c r="B29" s="2">
-        <v>7.5673831320259284</v>
+        <v>7.5673831320844851</v>
       </c>
       <c r="C29" s="2">
         <v>6.6999998092651367</v>
@@ -387,7 +387,7 @@
         <v>44682</v>
       </c>
       <c r="B30" s="2">
-        <v>6.8514983368694953</v>
+        <v>6.8514983348259006</v>
       </c>
       <c r="C30" s="2">
         <v>6</v>
@@ -398,7 +398,7 @@
         <v>44713</v>
       </c>
       <c r="B31" s="2">
-        <v>7.0988523981729088</v>
+        <v>7.098852398172915</v>
       </c>
       <c r="C31" s="2">
         <v>6</v>
@@ -409,10 +409,10 @@
         <v>44743</v>
       </c>
       <c r="B32" s="2">
-        <v>6.8909852014929864</v>
+        <v>6.8909852014929909</v>
       </c>
       <c r="C32" s="2">
-        <v>5.9000000953674317</v>
+        <v>5.9000000953674316</v>
       </c>
     </row>
     <row r="33">
@@ -530,7 +530,7 @@
         <v>45078</v>
       </c>
       <c r="B43" s="2">
-        <v>4.1854408428653311</v>
+        <v>4.185440842636833</v>
       </c>
       <c r="C43" s="2">
         <v>4</v>
@@ -552,10 +552,10 @@
         <v>45139</v>
       </c>
       <c r="B45" s="2">
-        <v>4.8853732058159514</v>
+        <v>4.885373206234223</v>
       </c>
       <c r="C45" s="2">
-        <v>4.9000000953674317</v>
+        <v>4.9000000953674316</v>
       </c>
     </row>
     <row r="46">
@@ -574,7 +574,7 @@
         <v>45200</v>
       </c>
       <c r="B47" s="2">
-        <v>5.0584100961271839</v>
+        <v>5.0584100961271883</v>
       </c>
       <c r="C47" s="2">
         <v>5</v>
@@ -585,7 +585,7 @@
         <v>45231</v>
       </c>
       <c r="B48" s="2">
-        <v>4.5508108925569211</v>
+        <v>4.5508108926848321</v>
       </c>
       <c r="C48" s="2">
         <v>4</v>
@@ -596,7 +596,7 @@
         <v>45261</v>
       </c>
       <c r="B49" s="2">
-        <v>4.4845725039920819</v>
+        <v>4.4845725047123643</v>
       </c>
       <c r="C49" s="2">
         <v>3.5</v>
@@ -618,7 +618,7 @@
         <v>45323</v>
       </c>
       <c r="B51" s="2">
-        <v>4.6070537224258068</v>
+        <v>4.6070537216546565</v>
       </c>
       <c r="C51" s="2">
         <v>3.5</v>
@@ -629,7 +629,7 @@
         <v>45352</v>
       </c>
       <c r="B52" s="2">
-        <v>4.3897269614028165</v>
+        <v>4.3897269615596946</v>
       </c>
       <c r="C52" s="2">
         <v>3.5</v>
@@ -640,7 +640,7 @@
         <v>45383</v>
       </c>
       <c r="B53" s="2">
-        <v>4.7483059676778821</v>
+        <v>4.748305967677882</v>
       </c>
       <c r="C53" s="2">
         <v>3.5</v>
@@ -672,15 +672,100 @@
       <c r="A56" s="1">
         <v>45474</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="B56" s="2">
+        <v>3.9907570458550135</v>
+      </c>
+      <c r="C56" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1">
         <v>45505</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="B57" s="2">
+        <v>4.0688963111175429</v>
+      </c>
+      <c r="C57" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1">
+        <v>45536</v>
+      </c>
+      <c r="B58" s="2">
+        <v>3.6999880014156212</v>
+      </c>
+      <c r="C58" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1">
+        <v>45566</v>
+      </c>
+      <c r="B59" s="2">
+        <v>4.1292384551086423</v>
+      </c>
+      <c r="C59" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1">
+        <v>45597</v>
+      </c>
+      <c r="B60" s="2">
+        <v>4.5625838084259742</v>
+      </c>
+      <c r="C60" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1">
+        <v>45627</v>
+      </c>
+      <c r="B61" s="2">
+        <v>4.4608988906167895</v>
+      </c>
+      <c r="C61" s="2">
+        <v>3.2000000476837158</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1">
+        <v>45658</v>
+      </c>
+      <c r="B62" s="2">
+        <v>4.337500418946691</v>
+      </c>
+      <c r="C62" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1">
+        <v>45689</v>
+      </c>
+      <c r="B63" s="2">
+        <v>4.8187867992992315</v>
+      </c>
+      <c r="C63" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1">
+        <v>45717</v>
+      </c>
+      <c r="B64" s="2">
+        <v>4.5453821191276251</v>
+      </c>
+      <c r="C64" s="2">
+        <v>3.5</v>
+      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>